<commit_message>
Changed name train visual widget to track visual widget, fixed switch error in the track layout json file
</commit_message>
<xml_diff>
--- a/system_data/tracks/green_line.xlsx
+++ b/system_data/tracks/green_line.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/tracks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7CE2D25-5DBC-4A7C-8949-A7280CCFC0CE}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3E7E1DB-C644-48AF-BB1A-85ED875C59B5}"/>
   <bookViews>
     <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="91">
   <si>
     <t>Section</t>
   </si>
@@ -270,9 +270,6 @@
     <t>1, 11, 13</t>
   </si>
   <si>
-    <t>27, 29, 150</t>
-  </si>
-  <si>
     <t>75, 77, 101</t>
   </si>
   <si>
@@ -295,6 +292,12 @@
   </si>
   <si>
     <t>1, 12</t>
+  </si>
+  <si>
+    <t>30, 150</t>
+  </si>
+  <si>
+    <t>29, 31, 150</t>
   </si>
 </sst>
 </file>
@@ -667,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -706,10 +709,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>67</v>
@@ -1264,7 +1267,7 @@
         <v>30</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
@@ -1303,7 +1306,11 @@
         <v>70</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f t="shared" ref="G15:G28" si="6">C14 &amp; ", " &amp; C16</f>
+        <f t="shared" ref="G15:G29" si="6">C14 &amp; ", " &amp; C16</f>
+        <v>13, 15</v>
+      </c>
+      <c r="I15" s="3" t="str">
+        <f>G15</f>
         <v>13, 15</v>
       </c>
       <c r="M15" s="3">
@@ -1343,6 +1350,10 @@
         <f t="shared" si="6"/>
         <v>14, 16</v>
       </c>
+      <c r="I16" s="3" t="str">
+        <f t="shared" ref="I16:I27" si="7">G16</f>
+        <v>14, 16</v>
+      </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1380,6 +1391,10 @@
         <f t="shared" si="6"/>
         <v>15, 17</v>
       </c>
+      <c r="I17" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>15, 17</v>
+      </c>
       <c r="J17" s="3" t="s">
         <v>67</v>
       </c>
@@ -1426,6 +1441,10 @@
         <f t="shared" si="6"/>
         <v>16, 18</v>
       </c>
+      <c r="I18" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>16, 18</v>
+      </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1463,6 +1482,10 @@
         <f t="shared" si="6"/>
         <v>17, 19</v>
       </c>
+      <c r="I19" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>17, 19</v>
+      </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1500,6 +1523,10 @@
         <f t="shared" si="6"/>
         <v>18, 20</v>
       </c>
+      <c r="I20" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>18, 20</v>
+      </c>
       <c r="K20" s="7" t="s">
         <v>49</v>
       </c>
@@ -1540,6 +1567,10 @@
         <f t="shared" si="6"/>
         <v>19, 21</v>
       </c>
+      <c r="I21" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>19, 21</v>
+      </c>
       <c r="M21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1577,6 +1608,10 @@
         <f t="shared" si="6"/>
         <v>20, 22</v>
       </c>
+      <c r="I22" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>20, 22</v>
+      </c>
       <c r="M22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1614,6 +1649,10 @@
         <f t="shared" si="6"/>
         <v>21, 23</v>
       </c>
+      <c r="I23" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>21, 23</v>
+      </c>
       <c r="J23" s="3" t="s">
         <v>70</v>
       </c>
@@ -1660,6 +1699,10 @@
         <f t="shared" si="6"/>
         <v>22, 24</v>
       </c>
+      <c r="I24" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>22, 24</v>
+      </c>
       <c r="M24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1697,6 +1740,10 @@
         <f t="shared" si="6"/>
         <v>23, 25</v>
       </c>
+      <c r="I25" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>23, 25</v>
+      </c>
       <c r="M25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1734,6 +1781,10 @@
         <f t="shared" si="6"/>
         <v>24, 26</v>
       </c>
+      <c r="I26" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>24, 26</v>
+      </c>
       <c r="M26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1771,6 +1822,10 @@
         <f t="shared" si="6"/>
         <v>25, 27</v>
       </c>
+      <c r="I27" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>25, 27</v>
+      </c>
       <c r="M27" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1808,6 +1863,10 @@
         <f t="shared" si="6"/>
         <v>26, 28</v>
       </c>
+      <c r="I28" s="3" t="str">
+        <f>G28</f>
+        <v>26, 28</v>
+      </c>
       <c r="M28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1841,8 +1900,9 @@
       <c r="F29" s="3">
         <v>30</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>81</v>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>27, 29</v>
       </c>
       <c r="M29" s="3">
         <f t="shared" si="0"/>
@@ -1880,6 +1940,9 @@
       <c r="G30" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="H30" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="K30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1916,9 +1979,8 @@
       <c r="F31" s="3">
         <v>30</v>
       </c>
-      <c r="G31" s="3" t="str">
-        <f t="shared" ref="G31:G76" si="7">C30 &amp; ", " &amp; C32</f>
-        <v>29, 31</v>
+      <c r="G31" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="M31" s="3">
         <f t="shared" si="0"/>
@@ -1954,7 +2016,7 @@
         <v>30</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="G31:G76" si="8">C31 &amp; ", " &amp; C33</f>
         <v>30, 32</v>
       </c>
       <c r="J32" s="3" t="s">
@@ -2000,7 +2062,7 @@
         <v>30</v>
       </c>
       <c r="G33" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>31, 33</v>
       </c>
       <c r="M33" s="3">
@@ -2037,11 +2099,11 @@
         <v>30</v>
       </c>
       <c r="G34" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>32, 34</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" ref="M34:M65" si="8">E34*D34/100</f>
+        <f t="shared" ref="M34:M65" si="9">E34*D34/100</f>
         <v>0</v>
       </c>
       <c r="N34" s="3">
@@ -2049,7 +2111,7 @@
         <v>0.5</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" ref="O34:O65" si="9">D34*(1/(F34*1000/(60*60)))</f>
+        <f t="shared" ref="O34:O65" si="10">D34*(1/(F34*1000/(60*60)))</f>
         <v>6</v>
       </c>
     </row>
@@ -2074,11 +2136,11 @@
         <v>30</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>33, 35</v>
       </c>
       <c r="M35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N35" s="3">
@@ -2086,7 +2148,7 @@
         <v>0.5</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2111,11 +2173,11 @@
         <v>30</v>
       </c>
       <c r="G36" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>34, 36</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N36" s="3">
@@ -2123,7 +2185,7 @@
         <v>0.5</v>
       </c>
       <c r="O36" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2148,14 +2210,14 @@
         <v>30</v>
       </c>
       <c r="G37" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35, 37</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N37" s="3">
@@ -2163,7 +2225,7 @@
         <v>0.5</v>
       </c>
       <c r="O37" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2188,14 +2250,14 @@
         <v>30</v>
       </c>
       <c r="G38" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36, 38</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M38" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N38" s="3">
@@ -2203,7 +2265,7 @@
         <v>0.5</v>
       </c>
       <c r="O38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2228,14 +2290,14 @@
         <v>30</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37, 39</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M39" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N39" s="3">
@@ -2243,7 +2305,7 @@
         <v>0.5</v>
       </c>
       <c r="O39" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2268,7 +2330,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>38, 40</v>
       </c>
       <c r="J40" s="3" t="s">
@@ -2281,7 +2343,7 @@
         <v>55</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N40" s="3">
@@ -2289,7 +2351,7 @@
         <v>0.5</v>
       </c>
       <c r="O40" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2314,14 +2376,14 @@
         <v>30</v>
       </c>
       <c r="G41" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>39, 41</v>
       </c>
       <c r="K41" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N41" s="3">
@@ -2329,7 +2391,7 @@
         <v>0.5</v>
       </c>
       <c r="O41" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2354,14 +2416,14 @@
         <v>30</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>40, 42</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N42" s="3">
@@ -2369,7 +2431,7 @@
         <v>0.5</v>
       </c>
       <c r="O42" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2394,14 +2456,14 @@
         <v>30</v>
       </c>
       <c r="G43" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>41, 43</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N43" s="3">
@@ -2409,7 +2471,7 @@
         <v>0.5</v>
       </c>
       <c r="O43" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2434,14 +2496,14 @@
         <v>30</v>
       </c>
       <c r="G44" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>42, 44</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M44" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N44" s="3">
@@ -2449,7 +2511,7 @@
         <v>0.5</v>
       </c>
       <c r="O44" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2474,14 +2536,14 @@
         <v>30</v>
       </c>
       <c r="G45" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>43, 45</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M45" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N45" s="3">
@@ -2489,7 +2551,7 @@
         <v>0.5</v>
       </c>
       <c r="O45" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2514,14 +2576,14 @@
         <v>30</v>
       </c>
       <c r="G46" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44, 46</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M46" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N46" s="3">
@@ -2529,7 +2591,7 @@
         <v>0.5</v>
       </c>
       <c r="O46" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2554,14 +2616,14 @@
         <v>30</v>
       </c>
       <c r="G47" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>45, 47</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M47" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N47" s="3">
@@ -2569,7 +2631,7 @@
         <v>0.5</v>
       </c>
       <c r="O47" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2594,14 +2656,14 @@
         <v>30</v>
       </c>
       <c r="G48" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>46, 48</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M48" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N48" s="3">
@@ -2609,7 +2671,7 @@
         <v>0.5</v>
       </c>
       <c r="O48" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2634,7 +2696,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>47, 49</v>
       </c>
       <c r="J49" s="3" t="s">
@@ -2647,7 +2709,7 @@
         <v>55</v>
       </c>
       <c r="M49" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N49" s="3">
@@ -2655,7 +2717,7 @@
         <v>0.5</v>
       </c>
       <c r="O49" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2680,14 +2742,14 @@
         <v>30</v>
       </c>
       <c r="G50" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>48, 50</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M50" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N50" s="3">
@@ -2695,7 +2757,7 @@
         <v>0.5</v>
       </c>
       <c r="O50" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2720,14 +2782,14 @@
         <v>30</v>
       </c>
       <c r="G51" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>49, 51</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M51" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N51" s="3">
@@ -2735,7 +2797,7 @@
         <v>0.5</v>
       </c>
       <c r="O51" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2760,14 +2822,14 @@
         <v>30</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50, 52</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M52" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N52" s="3">
@@ -2775,7 +2837,7 @@
         <v>0.5</v>
       </c>
       <c r="O52" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2800,14 +2862,14 @@
         <v>30</v>
       </c>
       <c r="G53" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>51, 53</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M53" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N53" s="3">
@@ -2815,7 +2877,7 @@
         <v>0.5</v>
       </c>
       <c r="O53" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2840,14 +2902,14 @@
         <v>30</v>
       </c>
       <c r="G54" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>52, 54</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M54" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N54" s="3">
@@ -2855,7 +2917,7 @@
         <v>0.5</v>
       </c>
       <c r="O54" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2880,14 +2942,14 @@
         <v>30</v>
       </c>
       <c r="G55" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>53, 55</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M55" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N55" s="3">
@@ -2895,7 +2957,7 @@
         <v>0.5</v>
       </c>
       <c r="O55" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2920,14 +2982,14 @@
         <v>30</v>
       </c>
       <c r="G56" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>54, 56</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M56" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N56" s="3">
@@ -2935,7 +2997,7 @@
         <v>0.5</v>
       </c>
       <c r="O56" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -2960,14 +3022,14 @@
         <v>30</v>
       </c>
       <c r="G57" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>55, 57</v>
       </c>
       <c r="K57" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M57" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N57" s="3">
@@ -2975,7 +3037,7 @@
         <v>0.5</v>
       </c>
       <c r="O57" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3000,7 +3062,7 @@
         <v>30</v>
       </c>
       <c r="G58" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56, 58</v>
       </c>
       <c r="J58" s="3" t="s">
@@ -3013,7 +3075,7 @@
         <v>55</v>
       </c>
       <c r="M58" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N58" s="3">
@@ -3021,7 +3083,7 @@
         <v>0.5</v>
       </c>
       <c r="O58" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3046,14 +3108,14 @@
         <v>30</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>57, 59</v>
       </c>
       <c r="K59" s="7" t="s">
         <v>58</v>
       </c>
       <c r="M59" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N59" s="3">
@@ -3061,7 +3123,7 @@
         <v>0.5</v>
       </c>
       <c r="O59" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3086,11 +3148,11 @@
         <v>30</v>
       </c>
       <c r="G60" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>58, 60</v>
       </c>
       <c r="M60" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N60" s="3">
@@ -3098,7 +3160,7 @@
         <v>0.5</v>
       </c>
       <c r="O60" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3123,11 +3185,11 @@
         <v>30</v>
       </c>
       <c r="G61" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>59, 61</v>
       </c>
       <c r="M61" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N61" s="3">
@@ -3135,7 +3197,7 @@
         <v>0.5</v>
       </c>
       <c r="O61" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3160,11 +3222,11 @@
         <v>30</v>
       </c>
       <c r="G62" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>60, 62</v>
       </c>
       <c r="M62" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N62" s="3">
@@ -3172,7 +3234,7 @@
         <v>0.5</v>
       </c>
       <c r="O62" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3197,14 +3259,14 @@
         <v>30</v>
       </c>
       <c r="G63" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>61, 63</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>59</v>
       </c>
       <c r="M63" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N63" s="3">
@@ -3212,7 +3274,7 @@
         <v>0.5</v>
       </c>
       <c r="O63" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -3237,11 +3299,11 @@
         <v>70</v>
       </c>
       <c r="G64" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>62, 64</v>
       </c>
       <c r="M64" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N64" s="3">
@@ -3249,7 +3311,7 @@
         <v>0.5</v>
       </c>
       <c r="O64" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.1428571428571432</v>
       </c>
     </row>
@@ -3274,11 +3336,11 @@
         <v>70</v>
       </c>
       <c r="G65" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>63, 65</v>
       </c>
       <c r="M65" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N65" s="3">
@@ -3286,7 +3348,7 @@
         <v>0.5</v>
       </c>
       <c r="O65" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.1428571428571432</v>
       </c>
     </row>
@@ -3311,7 +3373,7 @@
         <v>70</v>
       </c>
       <c r="G66" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>64, 66</v>
       </c>
       <c r="J66" s="3" t="s">
@@ -3324,7 +3386,7 @@
         <v>55</v>
       </c>
       <c r="M66" s="3">
-        <f t="shared" ref="M66:M97" si="10">E66*D66/100</f>
+        <f t="shared" ref="M66:M97" si="11">E66*D66/100</f>
         <v>0</v>
       </c>
       <c r="N66" s="3">
@@ -3332,7 +3394,7 @@
         <v>0.5</v>
       </c>
       <c r="O66" s="6">
-        <f t="shared" ref="O66:O97" si="11">D66*(1/(F66*1000/(60*60)))</f>
+        <f t="shared" ref="O66:O97" si="12">D66*(1/(F66*1000/(60*60)))</f>
         <v>10.285714285714286</v>
       </c>
     </row>
@@ -3357,11 +3419,11 @@
         <v>70</v>
       </c>
       <c r="G67" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>65, 67</v>
       </c>
       <c r="M67" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N67" s="3">
@@ -3369,13 +3431,13 @@
         <v>0.5</v>
       </c>
       <c r="O67" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.285714285714286</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="str">
-        <f t="shared" ref="A68:A131" si="12">A67</f>
+        <f t="shared" ref="A68:A131" si="13">A67</f>
         <v>Green</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -3394,25 +3456,25 @@
         <v>40</v>
       </c>
       <c r="G68" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>66, 68</v>
       </c>
       <c r="M68" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N68" s="3">
-        <f t="shared" ref="N68:N131" si="13">M68+N67</f>
+        <f t="shared" ref="N68:N131" si="14">M68+N67</f>
         <v>0.5</v>
       </c>
       <c r="O68" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -3431,25 +3493,25 @@
         <v>40</v>
       </c>
       <c r="G69" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>67, 69</v>
       </c>
       <c r="M69" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N69" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O69" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -3468,25 +3530,25 @@
         <v>40</v>
       </c>
       <c r="G70" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>68, 70</v>
       </c>
       <c r="M70" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N70" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -3505,25 +3567,25 @@
         <v>40</v>
       </c>
       <c r="G71" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>69, 71</v>
       </c>
       <c r="M71" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N71" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O71" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -3542,25 +3604,25 @@
         <v>40</v>
       </c>
       <c r="G72" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>70, 72</v>
       </c>
       <c r="M72" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N72" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O72" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -3579,25 +3641,25 @@
         <v>40</v>
       </c>
       <c r="G73" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>71, 73</v>
       </c>
       <c r="M73" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N73" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O73" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -3616,7 +3678,7 @@
         <v>40</v>
       </c>
       <c r="G74" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>72, 74</v>
       </c>
       <c r="J74" s="3" t="s">
@@ -3629,21 +3691,21 @@
         <v>55</v>
       </c>
       <c r="M74" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N74" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O74" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -3662,25 +3724,25 @@
         <v>40</v>
       </c>
       <c r="G75" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>73, 75</v>
       </c>
       <c r="M75" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N75" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O75" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -3699,25 +3761,25 @@
         <v>40</v>
       </c>
       <c r="G76" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>74, 76</v>
       </c>
       <c r="M76" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N76" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O76" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -3736,27 +3798,27 @@
         <v>40</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M77" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N77" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O77" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -3787,21 +3849,21 @@
         <v>48</v>
       </c>
       <c r="M78" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O78" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -3820,25 +3882,25 @@
         <v>70</v>
       </c>
       <c r="G79" s="3" t="str">
-        <f t="shared" ref="G79:G85" si="14">C78 &amp; ", " &amp; C80</f>
+        <f t="shared" ref="G79:G85" si="15">C78 &amp; ", " &amp; C80</f>
         <v>77, 79</v>
       </c>
       <c r="M79" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N79" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O79" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -3857,25 +3919,25 @@
         <v>70</v>
       </c>
       <c r="G80" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>78, 80</v>
+      </c>
+      <c r="M80" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N80" s="3">
         <f t="shared" si="14"/>
-        <v>78, 80</v>
-      </c>
-      <c r="M80" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N80" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O80" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -3894,25 +3956,25 @@
         <v>70</v>
       </c>
       <c r="G81" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>79, 81</v>
+      </c>
+      <c r="M81" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N81" s="3">
         <f t="shared" si="14"/>
-        <v>79, 81</v>
-      </c>
-      <c r="M81" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N81" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O81" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -3931,25 +3993,25 @@
         <v>70</v>
       </c>
       <c r="G82" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>80, 82</v>
+      </c>
+      <c r="M82" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N82" s="3">
         <f t="shared" si="14"/>
-        <v>80, 82</v>
-      </c>
-      <c r="M82" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N82" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O82" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -3968,25 +4030,25 @@
         <v>70</v>
       </c>
       <c r="G83" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>81, 83</v>
+      </c>
+      <c r="M83" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N83" s="3">
         <f t="shared" si="14"/>
-        <v>81, 83</v>
-      </c>
-      <c r="M83" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N83" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O83" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -4005,25 +4067,25 @@
         <v>70</v>
       </c>
       <c r="G84" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>82, 84</v>
+      </c>
+      <c r="M84" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N84" s="3">
         <f t="shared" si="14"/>
-        <v>82, 84</v>
-      </c>
-      <c r="M84" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N84" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O84" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -4042,25 +4104,25 @@
         <v>70</v>
       </c>
       <c r="G85" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>83, 85</v>
+      </c>
+      <c r="M85" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N85" s="3">
         <f t="shared" si="14"/>
-        <v>83, 85</v>
-      </c>
-      <c r="M85" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N85" s="3">
-        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="O85" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -4085,21 +4147,21 @@
         <v>64</v>
       </c>
       <c r="M86" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N86" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O86" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.428571428571431</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -4118,24 +4180,24 @@
         <v>25</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M87" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N87" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O87" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14.399999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -4154,25 +4216,25 @@
         <v>25</v>
       </c>
       <c r="G88" s="3" t="str">
-        <f t="shared" ref="G88:G100" si="15">C87 &amp; ", " &amp; C89</f>
+        <f t="shared" ref="G88:G100" si="16">C87 &amp; ", " &amp; C89</f>
         <v>86, 88</v>
       </c>
       <c r="M88" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N88" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O88" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.470399999999998</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -4191,7 +4253,7 @@
         <v>25</v>
       </c>
       <c r="G89" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>87, 89</v>
       </c>
       <c r="K89" s="7" t="s">
@@ -4201,21 +4263,21 @@
         <v>44</v>
       </c>
       <c r="M89" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N89" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O89" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14.399999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -4234,25 +4296,25 @@
         <v>25</v>
       </c>
       <c r="G90" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>88, 90</v>
       </c>
       <c r="M90" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.375</v>
       </c>
       <c r="N90" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.125</v>
       </c>
       <c r="O90" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -4271,25 +4333,25 @@
         <v>25</v>
       </c>
       <c r="G91" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>89, 91</v>
       </c>
       <c r="M91" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.75</v>
       </c>
       <c r="N91" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.625</v>
       </c>
       <c r="O91" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -4308,25 +4370,25 @@
         <v>25</v>
       </c>
       <c r="G92" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>90, 92</v>
       </c>
       <c r="M92" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.5</v>
       </c>
       <c r="N92" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2.125</v>
       </c>
       <c r="O92" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -4345,25 +4407,25 @@
         <v>25</v>
       </c>
       <c r="G93" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>91, 93</v>
       </c>
       <c r="M93" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N93" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2.125</v>
       </c>
       <c r="O93" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -4382,25 +4444,25 @@
         <v>25</v>
       </c>
       <c r="G94" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>92, 94</v>
       </c>
       <c r="M94" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="N94" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.625</v>
       </c>
       <c r="O94" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -4419,25 +4481,25 @@
         <v>25</v>
       </c>
       <c r="G95" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>93, 95</v>
       </c>
       <c r="M95" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="N95" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.125</v>
       </c>
       <c r="O95" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -4456,25 +4518,25 @@
         <v>25</v>
       </c>
       <c r="G96" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>94, 96</v>
       </c>
       <c r="M96" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.375</v>
       </c>
       <c r="N96" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O96" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -4493,7 +4555,7 @@
         <v>25</v>
       </c>
       <c r="G97" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>95, 97</v>
       </c>
       <c r="J97" s="3" t="s">
@@ -4506,21 +4568,21 @@
         <v>44</v>
       </c>
       <c r="M97" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N97" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O97" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -4539,25 +4601,25 @@
         <v>25</v>
       </c>
       <c r="G98" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>96, 98</v>
       </c>
       <c r="M98" s="3">
-        <f t="shared" ref="M98:M129" si="16">E98*D98/100</f>
+        <f t="shared" ref="M98:M129" si="17">E98*D98/100</f>
         <v>0</v>
       </c>
       <c r="N98" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O98" s="6">
-        <f t="shared" ref="O98:O129" si="17">D98*(1/(F98*1000/(60*60)))</f>
+        <f t="shared" ref="O98:O129" si="18">D98*(1/(F98*1000/(60*60)))</f>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -4576,25 +4638,25 @@
         <v>25</v>
       </c>
       <c r="G99" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>97, 99</v>
       </c>
       <c r="M99" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N99" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O99" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -4613,25 +4675,25 @@
         <v>25</v>
       </c>
       <c r="G100" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>98, 100</v>
       </c>
       <c r="M100" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N100" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O100" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -4650,24 +4712,24 @@
         <v>25</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M101" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N101" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O101" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.799999999999999</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -4686,24 +4748,24 @@
         <v>26</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M102" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N102" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O102" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.8461538461538467</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -4722,25 +4784,25 @@
         <v>28</v>
       </c>
       <c r="G103" s="3" t="str">
-        <f t="shared" ref="G103:G150" si="18">C102 &amp; ", " &amp; C104</f>
+        <f t="shared" ref="G103:G150" si="19">C102 &amp; ", " &amp; C104</f>
         <v>101, 103</v>
       </c>
       <c r="M103" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N103" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O103" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -4759,25 +4821,25 @@
         <v>28</v>
       </c>
       <c r="G104" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>102, 104</v>
+      </c>
+      <c r="M104" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N104" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O104" s="6">
         <f t="shared" si="18"/>
-        <v>102, 104</v>
-      </c>
-      <c r="M104" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N104" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O104" s="6">
-        <f t="shared" si="17"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -4796,25 +4858,25 @@
         <v>28</v>
       </c>
       <c r="G105" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>103, 105</v>
+      </c>
+      <c r="M105" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N105" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O105" s="6">
         <f t="shared" si="18"/>
-        <v>103, 105</v>
-      </c>
-      <c r="M105" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N105" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O105" s="6">
-        <f t="shared" si="17"/>
         <v>10.285714285714286</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -4833,7 +4895,7 @@
         <v>28</v>
       </c>
       <c r="G106" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>104, 106</v>
       </c>
       <c r="J106" s="3" t="s">
@@ -4847,21 +4909,21 @@
         <v>55</v>
       </c>
       <c r="M106" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N106" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O106" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -4880,25 +4942,25 @@
         <v>28</v>
       </c>
       <c r="G107" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>105, 107</v>
+      </c>
+      <c r="M107" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N107" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O107" s="6">
         <f t="shared" si="18"/>
-        <v>105, 107</v>
-      </c>
-      <c r="M107" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N107" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O107" s="6">
-        <f t="shared" si="17"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -4917,25 +4979,25 @@
         <v>28</v>
       </c>
       <c r="G108" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>106, 108</v>
+      </c>
+      <c r="M108" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N108" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O108" s="6">
         <f t="shared" si="18"/>
-        <v>106, 108</v>
-      </c>
-      <c r="M108" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N108" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O108" s="6">
-        <f t="shared" si="17"/>
         <v>11.571428571428573</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -4954,25 +5016,25 @@
         <v>28</v>
       </c>
       <c r="G109" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>107, 109</v>
+      </c>
+      <c r="M109" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N109" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O109" s="6">
         <f t="shared" si="18"/>
-        <v>107, 109</v>
-      </c>
-      <c r="M109" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N109" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O109" s="6">
-        <f t="shared" si="17"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -4991,25 +5053,25 @@
         <v>28</v>
       </c>
       <c r="G110" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>108, 110</v>
+      </c>
+      <c r="M110" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N110" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O110" s="6">
         <f t="shared" si="18"/>
-        <v>108, 110</v>
-      </c>
-      <c r="M110" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N110" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O110" s="6">
-        <f t="shared" si="17"/>
         <v>12.857142857142859</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -5028,25 +5090,25 @@
         <v>30</v>
       </c>
       <c r="G111" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>109, 111</v>
+      </c>
+      <c r="M111" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N111" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O111" s="6">
         <f t="shared" si="18"/>
-        <v>109, 111</v>
-      </c>
-      <c r="M111" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N111" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O111" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -5065,25 +5127,25 @@
         <v>30</v>
       </c>
       <c r="G112" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>110, 112</v>
+      </c>
+      <c r="M112" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N112" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O112" s="6">
         <f t="shared" si="18"/>
-        <v>110, 112</v>
-      </c>
-      <c r="M112" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N112" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O112" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -5102,25 +5164,25 @@
         <v>30</v>
       </c>
       <c r="G113" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>111, 113</v>
+      </c>
+      <c r="M113" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N113" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O113" s="6">
         <f t="shared" si="18"/>
-        <v>111, 113</v>
-      </c>
-      <c r="M113" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N113" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O113" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -5139,25 +5201,25 @@
         <v>30</v>
       </c>
       <c r="G114" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>112, 114</v>
+      </c>
+      <c r="M114" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N114" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O114" s="6">
         <f t="shared" si="18"/>
-        <v>112, 114</v>
-      </c>
-      <c r="M114" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N114" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O114" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -5177,7 +5239,7 @@
         <v>30</v>
       </c>
       <c r="G115" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>113, 115</v>
       </c>
       <c r="J115" s="3" t="s">
@@ -5191,21 +5253,21 @@
         <v>55</v>
       </c>
       <c r="M115" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N115" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O115" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>19.439999999999998</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B116" s="3" t="s">
@@ -5224,25 +5286,25 @@
         <v>30</v>
       </c>
       <c r="G116" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>114, 116</v>
+      </c>
+      <c r="M116" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N116" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O116" s="6">
         <f t="shared" si="18"/>
-        <v>114, 116</v>
-      </c>
-      <c r="M116" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N116" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O116" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -5261,25 +5323,25 @@
         <v>30</v>
       </c>
       <c r="G117" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>115, 117</v>
+      </c>
+      <c r="M117" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N117" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O117" s="6">
         <f t="shared" si="18"/>
-        <v>115, 117</v>
-      </c>
-      <c r="M117" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N117" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O117" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -5298,25 +5360,25 @@
         <v>15</v>
       </c>
       <c r="G118" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>116, 118</v>
+      </c>
+      <c r="M118" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N118" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O118" s="6">
         <f t="shared" si="18"/>
-        <v>116, 118</v>
-      </c>
-      <c r="M118" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N118" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O118" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -5335,25 +5397,25 @@
         <v>15</v>
       </c>
       <c r="G119" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>117, 119</v>
+      </c>
+      <c r="M119" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N119" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O119" s="6">
         <f t="shared" si="18"/>
-        <v>117, 119</v>
-      </c>
-      <c r="M119" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N119" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O119" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -5372,25 +5434,25 @@
         <v>15</v>
       </c>
       <c r="G120" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>118, 120</v>
+      </c>
+      <c r="M120" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N120" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O120" s="6">
         <f t="shared" si="18"/>
-        <v>118, 120</v>
-      </c>
-      <c r="M120" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N120" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O120" s="6">
-        <f t="shared" si="17"/>
         <v>9.6</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -5409,25 +5471,25 @@
         <v>15</v>
       </c>
       <c r="G121" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>119, 121</v>
+      </c>
+      <c r="M121" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N121" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O121" s="6">
         <f t="shared" si="18"/>
-        <v>119, 121</v>
-      </c>
-      <c r="M121" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N121" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O121" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -5446,25 +5508,25 @@
         <v>15</v>
       </c>
       <c r="G122" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>120, 122</v>
+      </c>
+      <c r="M122" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N122" s="3">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O122" s="6">
         <f t="shared" si="18"/>
-        <v>120, 122</v>
-      </c>
-      <c r="M122" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N122" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="O122" s="6">
-        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -5483,28 +5545,28 @@
         <v>20</v>
       </c>
       <c r="G123" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>121, 123</v>
       </c>
       <c r="K123" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M123" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N123" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O123" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -5523,7 +5585,7 @@
         <v>20</v>
       </c>
       <c r="G124" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>122, 124</v>
       </c>
       <c r="J124" s="3" t="s">
@@ -5537,21 +5599,21 @@
         <v>55</v>
       </c>
       <c r="M124" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N124" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O124" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -5570,28 +5632,28 @@
         <v>20</v>
       </c>
       <c r="G125" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>123, 125</v>
       </c>
       <c r="K125" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M125" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N125" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O125" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -5610,28 +5672,28 @@
         <v>20</v>
       </c>
       <c r="G126" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>124, 126</v>
       </c>
       <c r="K126" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M126" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N126" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O126" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -5650,28 +5712,28 @@
         <v>20</v>
       </c>
       <c r="G127" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>125, 127</v>
       </c>
       <c r="K127" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M127" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N127" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O127" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -5690,28 +5752,28 @@
         <v>20</v>
       </c>
       <c r="G128" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>126, 128</v>
       </c>
       <c r="K128" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M128" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N128" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O128" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
@@ -5730,28 +5792,28 @@
         <v>20</v>
       </c>
       <c r="G129" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>127, 129</v>
       </c>
       <c r="K129" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M129" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N129" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O129" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -5770,28 +5832,28 @@
         <v>20</v>
       </c>
       <c r="G130" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>128, 130</v>
       </c>
       <c r="K130" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M130" s="3">
-        <f t="shared" ref="M130:M151" si="19">E130*D130/100</f>
+        <f t="shared" ref="M130:M151" si="20">E130*D130/100</f>
         <v>0</v>
       </c>
       <c r="N130" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O130" s="6">
-        <f t="shared" ref="O130:O151" si="20">D130*(1/(F130*1000/(60*60)))</f>
+        <f t="shared" ref="O130:O151" si="21">D130*(1/(F130*1000/(60*60)))</f>
         <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -5810,28 +5872,28 @@
         <v>20</v>
       </c>
       <c r="G131" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>129, 131</v>
       </c>
       <c r="K131" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M131" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N131" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="O131" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="str">
-        <f t="shared" ref="A132:A151" si="21">A131</f>
+        <f t="shared" ref="A132:A151" si="22">A131</f>
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -5850,28 +5912,28 @@
         <v>20</v>
       </c>
       <c r="G132" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>130, 132</v>
       </c>
       <c r="K132" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M132" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N132" s="3">
-        <f t="shared" ref="N132:N151" si="22">M132+N131</f>
+        <f t="shared" ref="N132:N151" si="23">M132+N131</f>
         <v>0.5</v>
       </c>
       <c r="O132" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
@@ -5890,7 +5952,7 @@
         <v>20</v>
       </c>
       <c r="G133" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>131, 133</v>
       </c>
       <c r="J133" s="3" t="s">
@@ -5904,21 +5966,21 @@
         <v>44</v>
       </c>
       <c r="M133" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N133" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O133" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -5937,28 +5999,28 @@
         <v>20</v>
       </c>
       <c r="G134" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>132, 134</v>
       </c>
       <c r="K134" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M134" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N134" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O134" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -5977,28 +6039,28 @@
         <v>20</v>
       </c>
       <c r="G135" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>133, 135</v>
       </c>
       <c r="K135" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M135" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N135" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O135" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
@@ -6017,28 +6079,28 @@
         <v>20</v>
       </c>
       <c r="G136" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>134, 136</v>
       </c>
       <c r="K136" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M136" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N136" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O136" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -6057,28 +6119,28 @@
         <v>20</v>
       </c>
       <c r="G137" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>135, 137</v>
       </c>
       <c r="K137" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M137" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N137" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O137" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -6097,28 +6159,28 @@
         <v>20</v>
       </c>
       <c r="G138" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>136, 138</v>
       </c>
       <c r="K138" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M138" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N138" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O138" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -6137,28 +6199,28 @@
         <v>20</v>
       </c>
       <c r="G139" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>137, 139</v>
       </c>
       <c r="K139" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M139" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N139" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O139" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -6177,28 +6239,28 @@
         <v>20</v>
       </c>
       <c r="G140" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>138, 140</v>
       </c>
       <c r="K140" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M140" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N140" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O140" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
@@ -6217,28 +6279,28 @@
         <v>20</v>
       </c>
       <c r="G141" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>139, 141</v>
       </c>
       <c r="K141" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M141" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N141" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O141" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -6257,7 +6319,7 @@
         <v>20</v>
       </c>
       <c r="G142" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>140, 142</v>
       </c>
       <c r="J142" s="3" t="s">
@@ -6271,21 +6333,21 @@
         <v>55</v>
       </c>
       <c r="M142" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N142" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O142" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
@@ -6304,28 +6366,28 @@
         <v>20</v>
       </c>
       <c r="G143" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>141, 143</v>
       </c>
       <c r="K143" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M143" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N143" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O143" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -6344,28 +6406,28 @@
         <v>20</v>
       </c>
       <c r="G144" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>142, 144</v>
       </c>
       <c r="K144" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M144" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N144" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O144" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -6384,25 +6446,25 @@
         <v>20</v>
       </c>
       <c r="G145" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>143, 145</v>
       </c>
       <c r="M145" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N145" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O145" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -6421,25 +6483,25 @@
         <v>20</v>
       </c>
       <c r="G146" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>144, 146</v>
       </c>
       <c r="M146" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N146" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O146" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -6458,25 +6520,25 @@
         <v>20</v>
       </c>
       <c r="G147" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>145, 147</v>
       </c>
       <c r="M147" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N147" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O147" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -6495,25 +6557,25 @@
         <v>20</v>
       </c>
       <c r="G148" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>146, 148</v>
       </c>
       <c r="M148" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N148" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O148" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -6533,25 +6595,25 @@
         <v>20</v>
       </c>
       <c r="G149" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>147, 149</v>
       </c>
       <c r="M149" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N149" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O149" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33.119999999999997</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -6570,25 +6632,25 @@
         <v>20</v>
       </c>
       <c r="G150" s="3" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>148, 150</v>
       </c>
       <c r="M150" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N150" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O150" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7.1999999999999993</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -6607,18 +6669,18 @@
         <v>20</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M151" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N151" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="O151" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.3</v>
       </c>
     </row>

</xml_diff>